<commit_message>
Fixed the mismatch in some of the changed random events from last week and updated the stat table with the new events
</commit_message>
<xml_diff>
--- a/Assets/StatTable.xlsx
+++ b/Assets/StatTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityProject\ShadowsOfHuntshire\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordan/Desktop/ShadowsOfHuntshire/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBB6269-9DDF-4923-AA6A-BB7544883C39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD063502-2AED-9645-8062-504E1574012E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8F7BB208-E0CD-49C9-B2DA-F58E0459B174}"/>
+    <workbookView xWindow="-19200" yWindow="5460" windowWidth="20440" windowHeight="12580" xr2:uid="{8F7BB208-E0CD-49C9-B2DA-F58E0459B174}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Time</t>
   </si>
@@ -211,6 +220,36 @@
   </si>
   <si>
     <t>(All values should be &lt; 9!)</t>
+  </si>
+  <si>
+    <t>A Scurrying Racket 1</t>
+  </si>
+  <si>
+    <t>A Scurrying Racket 2</t>
+  </si>
+  <si>
+    <t>Deepening Chill 1</t>
+  </si>
+  <si>
+    <t>Deepening Chill 2</t>
+  </si>
+  <si>
+    <t>Unknown Chuckle 1</t>
+  </si>
+  <si>
+    <t>Unknown Chuckle 2</t>
+  </si>
+  <si>
+    <t>Withered Petals 1</t>
+  </si>
+  <si>
+    <t>Withered Petals 2</t>
+  </si>
+  <si>
+    <t>Liquid Yearning 1</t>
+  </si>
+  <si>
+    <t>Liquid Yearning 2</t>
   </si>
 </sst>
 </file>
@@ -573,22 +612,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974DC328-D1FF-4833-BC5C-D56949842991}">
-  <dimension ref="C3:Z45"/>
+  <dimension ref="C3:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="10" max="12" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="10" max="12" width="12.5" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:26" x14ac:dyDescent="0.2">
       <c r="N3" s="5" t="s">
         <v>60</v>
       </c>
@@ -600,7 +639,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -653,7 +692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>0</v>
       </c>
@@ -686,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>0</v>
       </c>
@@ -742,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>0</v>
       </c>
@@ -800,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>0</v>
       </c>
@@ -856,7 +895,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>0</v>
       </c>
@@ -921,7 +960,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>2</v>
       </c>
@@ -951,15 +990,15 @@
       </c>
       <c r="N10" s="4">
         <f>J10+(($C10*J$26*2)/COUNT(F$5:F10))</f>
-        <v>9.3666666666666654</v>
+        <v>9.5111111111111111</v>
       </c>
       <c r="O10" s="4">
         <f>K10+(($C10*K$26*2)/COUNT(G$5:G10))</f>
-        <v>9.1000000000000014</v>
+        <v>9.1555555555555568</v>
       </c>
       <c r="P10" s="4">
         <f>L10+(($C10*L$26*2)/COUNT(H$5:H10))</f>
-        <v>5.7666666666666666</v>
+        <v>5.8666666666666663</v>
       </c>
       <c r="T10">
         <f t="shared" si="0"/>
@@ -986,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>5</v>
       </c>
@@ -1042,7 +1081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>5</v>
       </c>
@@ -1072,15 +1111,15 @@
       </c>
       <c r="N12" s="4">
         <f>J12+(($C12*J$26*2)/COUNT(F$5:F12))</f>
-        <v>8.8125</v>
+        <v>9.0833333333333339</v>
       </c>
       <c r="O12" s="4">
         <f>K12+(($C12*K$26*2)/COUNT(G$5:G12))</f>
-        <v>10.1875</v>
+        <v>10.291666666666666</v>
       </c>
       <c r="P12" s="4">
         <f>L12+(($C12*L$26*2)/COUNT(H$5:H12))</f>
-        <v>7.0625</v>
+        <v>7.25</v>
       </c>
       <c r="T12">
         <f t="shared" si="0"/>
@@ -1107,7 +1146,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>9</v>
       </c>
@@ -1137,15 +1176,15 @@
       </c>
       <c r="N13" s="4">
         <f>J13+(($C13*J$26*2)/COUNT(F$5:F13))</f>
-        <v>7.8777777777777782</v>
+        <v>8.3111111111111118</v>
       </c>
       <c r="O13" s="4">
         <f>K13+(($C13*K$26*2)/COUNT(G$5:G13))</f>
-        <v>9.8555555555555561</v>
+        <v>10.022222222222222</v>
       </c>
       <c r="P13" s="4">
         <f>L13+(($C13*L$26*2)/COUNT(H$5:H13))</f>
-        <v>8.6333333333333346</v>
+        <v>8.9333333333333336</v>
       </c>
       <c r="T13">
         <f t="shared" si="0"/>
@@ -1172,7 +1211,7 @@
         <v>5.5555555555555554</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>13</v>
       </c>
@@ -1202,15 +1241,15 @@
       </c>
       <c r="N14" s="4">
         <f>J14+(($C14*J$26*2)/COUNT(F$5:F14))</f>
-        <v>7.6300000000000008</v>
+        <v>8.1933333333333334</v>
       </c>
       <c r="O14" s="4">
         <f>K14+(($C14*K$26*2)/COUNT(G$5:G14))</f>
-        <v>8.89</v>
+        <v>9.1066666666666674</v>
       </c>
       <c r="P14" s="4">
         <f>L14+(($C14*L$26*2)/COUNT(H$5:H14))</f>
-        <v>9.49</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="T14">
         <f t="shared" si="0"/>
@@ -1237,7 +1276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>17</v>
       </c>
@@ -1267,15 +1306,15 @@
       </c>
       <c r="N15" s="4">
         <f>J15+(($C15*J$26*2)/COUNT(F$5:F15))</f>
-        <v>8.4272727272727277</v>
+        <v>9.0969696969696976</v>
       </c>
       <c r="O15" s="4">
         <f>K15+(($C15*K$26*2)/COUNT(G$5:G15))</f>
-        <v>8.5545454545454547</v>
+        <v>8.8121212121212125</v>
       </c>
       <c r="P15" s="4">
         <f>L15+(($C15*L$26*2)/COUNT(H$5:H15))</f>
-        <v>9.1</v>
+        <v>9.5636363636363626</v>
       </c>
       <c r="T15">
         <f t="shared" si="0"/>
@@ -1302,7 +1341,7 @@
         <v>5.6363636363636367</v>
       </c>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>21</v>
       </c>
@@ -1332,15 +1371,15 @@
       </c>
       <c r="N16" s="4">
         <f>J16+(($C16*J$26*2)/COUNT(F$5:F16))</f>
-        <v>8.091666666666665</v>
+        <v>8.85</v>
       </c>
       <c r="O16" s="4">
         <f>K16+(($C16*K$26*2)/COUNT(G$5:G16))</f>
-        <v>9.2750000000000004</v>
+        <v>9.5666666666666664</v>
       </c>
       <c r="P16" s="4">
         <f>L16+(($C16*L$26*2)/COUNT(H$5:H16))</f>
-        <v>8.7750000000000004</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="T16">
         <f t="shared" si="0"/>
@@ -1367,7 +1406,7 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>21</v>
       </c>
@@ -1423,7 +1462,7 @@
         <v>5.6923076923076925</v>
       </c>
     </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>25</v>
       </c>
@@ -1453,15 +1492,15 @@
       </c>
       <c r="N18" s="4">
         <f>J18+(($C18*J$26*2)/COUNT(F$5:F18))</f>
-        <v>8.3928571428571423</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="O18" s="4">
         <f>K18+(($C18*K$26*2)/COUNT(G$5:G18))</f>
-        <v>8.3928571428571423</v>
+        <v>8.6904761904761898</v>
       </c>
       <c r="P18" s="4">
         <f>L18+(($C18*L$26*2)/COUNT(H$5:H18))</f>
-        <v>9.3928571428571423</v>
+        <v>9.9285714285714288</v>
       </c>
       <c r="T18">
         <f t="shared" si="0"/>
@@ -1488,7 +1527,7 @@
         <v>5.3571428571428568</v>
       </c>
     </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>25</v>
       </c>
@@ -1544,7 +1583,7 @@
         <v>5.2666666666666666</v>
       </c>
     </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>33</v>
       </c>
@@ -1574,15 +1613,15 @@
       </c>
       <c r="N20" s="4">
         <f>J20+(($C20*J$26*2)/COUNT(F$5:F20))</f>
-        <v>7.7687499999999998</v>
+        <v>8.6624999999999996</v>
       </c>
       <c r="O20" s="4">
         <f>K20+(($C20*K$26*2)/COUNT(G$5:G20))</f>
-        <v>7.8687500000000004</v>
+        <v>8.2125000000000004</v>
       </c>
       <c r="P20" s="4">
         <f>L20+(($C20*L$26*2)/COUNT(H$5:H20))</f>
-        <v>8.6187500000000004</v>
+        <v>9.2375000000000007</v>
       </c>
       <c r="T20">
         <f t="shared" si="0"/>
@@ -1609,7 +1648,7 @@
         <v>5.1875</v>
       </c>
     </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>37</v>
       </c>
@@ -1639,15 +1678,15 @@
       </c>
       <c r="N21" s="4">
         <f>J21+(($C21*J$26*2)/COUNT(F$5:F21))</f>
-        <v>8.1</v>
+        <v>9.0431372549019606</v>
       </c>
       <c r="O21" s="4">
         <f>K21+(($C21*K$26*2)/COUNT(G$5:G21))</f>
-        <v>8.7117647058823522</v>
+        <v>9.0745098039215684</v>
       </c>
       <c r="P21" s="4">
         <f>L21+(($C21*L$26*2)/COUNT(H$5:H21))</f>
-        <v>8.7117647058823522</v>
+        <v>9.3647058823529399</v>
       </c>
       <c r="T21">
         <f t="shared" si="0"/>
@@ -1674,12 +1713,12 @@
         <v>5.0588235294117645</v>
       </c>
     </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:26" x14ac:dyDescent="0.2">
       <c r="J24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>32</v>
       </c>
@@ -1702,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>36</v>
       </c>
@@ -1716,19 +1755,19 @@
         <v>-2</v>
       </c>
       <c r="J26" s="3">
-        <f>AVERAGE(F26:F45)</f>
-        <v>-0.45</v>
+        <f>AVERAGE(F26:F55)</f>
+        <v>-0.23333333333333334</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" ref="K26:L26" si="3">AVERAGE(G26:G45)</f>
-        <v>-0.35</v>
+        <f>AVERAGE(G26:G55)</f>
+        <v>-0.26666666666666666</v>
       </c>
       <c r="L26" s="3">
-        <f>AVERAGE(H26:H45)</f>
-        <v>-0.35</v>
-      </c>
-    </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+        <f>AVERAGE(H26:H55)</f>
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>37</v>
       </c>
@@ -1742,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>38</v>
       </c>
@@ -1756,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>39</v>
       </c>
@@ -1770,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>40</v>
       </c>
@@ -1784,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>41</v>
       </c>
@@ -1798,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:26" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
         <v>42</v>
       </c>
@@ -1812,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>43</v>
       </c>
@@ -1826,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>44</v>
       </c>
@@ -1840,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>45</v>
       </c>
@@ -1854,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>46</v>
       </c>
@@ -1868,7 +1907,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>47</v>
       </c>
@@ -1882,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>48</v>
       </c>
@@ -1896,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
         <v>49</v>
       </c>
@@ -1910,7 +1949,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>50</v>
       </c>
@@ -1924,12 +1963,12 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
         <v>51</v>
       </c>
       <c r="F41">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1938,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>52</v>
       </c>
@@ -1952,7 +1991,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
         <v>53</v>
       </c>
@@ -1966,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
         <v>54</v>
       </c>
@@ -1980,7 +2019,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
         <v>55</v>
       </c>
@@ -1992,6 +2031,146 @@
       </c>
       <c r="H45">
         <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47">
+        <v>-2</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>65</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>-1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>-2</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>68</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>-1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54">
+        <v>-3</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>71</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>-2</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>